<commit_message>
[ ADD  ] Test/Test_Training_Result.xlsx          best.onnx files (Model Outputs) [Update] ResearchNote.docx
</commit_message>
<xml_diff>
--- a/1.PrecisionLandingModule/2.Version_1.0/3.LandingStation/1.Src/1. YOLOv8_detect_drones_model/Test/Test_Training_Result.xlsx
+++ b/1.PrecisionLandingModule/2.Version_1.0/3.LandingStation/1.Src/1. YOLOv8_detect_drones_model/Test/Test_Training_Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvvsk\Desktop\Git\Capstone_Design\1.PrecisionLandingModule\2.Version_1.0\3.LandingStation\1.Src\1. YOLOv8_detect_drones_model\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D4204B-5763-4A3D-9F42-5486B059DAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76D1359-A0AB-4ECA-BFE9-5EA31261C966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="3640" windowWidth="28800" windowHeight="15370" xr2:uid="{9CE10038-FE34-4213-AD70-C96AAAD0B212}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9CE10038-FE34-4213-AD70-C96AAAD0B212}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>2025_03_23</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,12 +103,16 @@
   <si>
     <t>Box(P</t>
   </si>
+  <si>
+    <t>Realtime YoloV8n detection drone sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +131,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -263,7 +276,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -275,6 +288,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -288,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -303,14 +325,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,7 +411,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1500,6 +1516,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381002</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>121479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>320260</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>53961</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A361DBD-CD82-E22C-2483-A0535EAB0013}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16184219" y="1203740"/>
+          <a:ext cx="3252302" cy="2085960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1802,10 +1862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493BE305-66FE-4D4D-A743-49714564E832}">
-  <dimension ref="B4:U16"/>
+  <dimension ref="B3:AC16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1816,65 +1876,87 @@
     <col min="21" max="21" width="11.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="I4" s="15" t="s">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="X3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="I4" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
     </row>
-    <row r="5" spans="2:21" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
+    <row r="5" spans="2:29" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="9"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="I7" s="13" t="s">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1913,15 +1995,21 @@
       <c r="U7" s="1">
         <v>0.316</v>
       </c>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="12"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="I8" s="13" t="s">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1960,15 +2048,21 @@
       <c r="U8" s="1">
         <v>0.36199999999999999</v>
       </c>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="12"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="I9" s="13" t="s">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="I9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -2007,15 +2101,21 @@
       <c r="U9" s="1">
         <v>0.36799999999999999</v>
       </c>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="12"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="I10" s="13" t="s">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="I10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -2054,15 +2154,21 @@
       <c r="U10" s="1">
         <v>0.38300000000000001</v>
       </c>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="12"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="I11" s="13" t="s">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="I11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -2101,15 +2207,21 @@
       <c r="U11" s="1">
         <v>0.436</v>
       </c>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="12"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="I12" s="13" t="s">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="I12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -2148,15 +2260,21 @@
       <c r="U12" s="1">
         <v>0.44700000000000001</v>
       </c>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="12"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="I13" s="13" t="s">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="I13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -2195,15 +2313,21 @@
       <c r="U13" s="1">
         <v>0.45700000000000002</v>
       </c>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="12"/>
     </row>
-    <row r="14" spans="2:21" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="I14" s="13" t="s">
+    <row r="14" spans="2:29" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="I14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -2242,15 +2366,21 @@
       <c r="U14" s="1">
         <v>0.48899999999999999</v>
       </c>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="12"/>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="I15" s="13" t="s">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="I15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J15" s="1"/>
@@ -2265,15 +2395,21 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="12"/>
     </row>
-    <row r="16" spans="2:21" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="I16" s="13" t="s">
+    <row r="16" spans="2:29" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="I16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J16" s="1"/>
@@ -2288,13 +2424,22 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B6:G16"/>
+    <mergeCell ref="X6:AC16"/>
+    <mergeCell ref="X3:AC4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>